<commit_message>
Updated for Theory and Lab Periods
</commit_message>
<xml_diff>
--- a/Proyecto/data/profesores.xlsx
+++ b/Proyecto/data/profesores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UVG\Final Round\Tesis\Prubeas\Git\TG2018\Proyecto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BC1FFD-B3E0-4758-B7AD-5D81F1A8B431}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5EB1A0-487D-41BE-B429-85DF60387AC8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" activeTab="2" xr2:uid="{13BC5F08-0E1E-4337-855E-932CC9DF5409}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="32">
   <si>
     <t>No. Per.</t>
   </si>
@@ -111,14 +111,32 @@
     <t>IE3048</t>
   </si>
   <si>
-    <t>MM2039</t>
+    <t>IE2010</t>
+  </si>
+  <si>
+    <t>IE2008</t>
+  </si>
+  <si>
+    <t>IE2016</t>
+  </si>
+  <si>
+    <t>IE3028</t>
+  </si>
+  <si>
+    <t>IE2011</t>
+  </si>
+  <si>
+    <t>IE2009</t>
+  </si>
+  <si>
+    <t>IE2013</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,16 +160,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -284,30 +292,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -504,19 +488,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -539,69 +510,102 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -611,7 +615,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -628,43 +632,85 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="3" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -673,175 +719,64 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1160,8 +1095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{098A41C1-A973-4B3A-9E26-E4499DF2AB67}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,61 +1107,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="73" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="74"/>
-      <c r="K1" s="75"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="30"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="24" t="s">
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="71" t="s">
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="72" t="s">
+      <c r="J2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="72" t="s">
+      <c r="K2" s="27" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="24" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1253,9 +1188,9 @@
       <c r="H4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -1267,19 +1202,29 @@
       <c r="C5" s="4">
         <v>0.32291666666666669</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="60" t="s">
+      <c r="D5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="76">
+      <c r="J5" s="22">
         <v>1</v>
       </c>
-      <c r="K5" s="61">
-        <v>0</v>
+      <c r="K5" s="18">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1292,18 +1237,28 @@
       <c r="C6" s="4">
         <v>0.3576388888888889</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="63" t="s">
+      <c r="D6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="40">
-        <v>2</v>
-      </c>
-      <c r="K6" s="41">
+      <c r="J6" s="8">
+        <v>1</v>
+      </c>
+      <c r="K6" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1317,19 +1272,29 @@
       <c r="C7" s="4">
         <v>0.3923611111111111</v>
       </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="40">
+      <c r="D7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="8">
         <v>1</v>
       </c>
-      <c r="K7" s="41">
-        <v>2</v>
+      <c r="K7" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1342,24 +1307,30 @@
       <c r="C8" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="D8" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="63"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="41"/>
+      <c r="D8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="8">
+        <v>2</v>
+      </c>
+      <c r="K8" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1371,14 +1342,14 @@
       <c r="C9" s="4">
         <v>0.44444444444444442</v>
       </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="41"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -1390,14 +1361,24 @@
       <c r="C10" s="4">
         <v>0.47569444444444442</v>
       </c>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="63"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="41"/>
+      <c r="D10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="19"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -1409,14 +1390,24 @@
       <c r="C11" s="4">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="41"/>
+      <c r="D11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="19"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="9"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -1428,14 +1419,24 @@
       <c r="C12" s="4">
         <v>0.54513888888888895</v>
       </c>
-      <c r="D12" s="31"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="63"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="41"/>
+      <c r="D12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="19"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="9"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -1447,14 +1448,14 @@
       <c r="C13" s="4">
         <v>0.57986111111111105</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="41"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -1466,14 +1467,14 @@
       <c r="C14" s="4">
         <v>0.61458333333333337</v>
       </c>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="63"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="41"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="9"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -1485,14 +1486,14 @@
       <c r="C15" s="4">
         <v>0.64930555555555558</v>
       </c>
-      <c r="D15" s="31"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="41"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -1504,14 +1505,14 @@
       <c r="C16" s="4">
         <v>0.68402777777777779</v>
       </c>
-      <c r="D16" s="29"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="63"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="41"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="9"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -1523,14 +1524,14 @@
       <c r="C17" s="4">
         <v>0.71875</v>
       </c>
-      <c r="D17" s="31"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="63"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="41"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="9"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -1542,14 +1543,14 @@
       <c r="C18" s="4">
         <v>0.75347222222222221</v>
       </c>
-      <c r="D18" s="34"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="63"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="41"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="9"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -1561,24 +1562,14 @@
       <c r="C19" s="4">
         <v>0.78819444444444453</v>
       </c>
-      <c r="D19" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="I19" s="63"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="41"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="9"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -1590,27 +1581,17 @@
       <c r="C20" s="4">
         <v>0.82291666666666663</v>
       </c>
-      <c r="D20" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="I20" s="63"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="41"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="9"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="53">
+      <c r="A21" s="15">
         <v>16</v>
       </c>
       <c r="B21" s="4">
@@ -1619,51 +1600,33 @@
       <c r="C21" s="4">
         <v>0.85763888888888884</v>
       </c>
-      <c r="D21" s="66"/>
-      <c r="E21" s="66" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="66" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="66" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="63"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="41"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="9"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="47">
+      <c r="A22" s="11">
         <v>17</v>
       </c>
-      <c r="B22" s="48">
+      <c r="B22" s="12">
         <v>0.86111111111111116</v>
       </c>
-      <c r="C22" s="48">
+      <c r="C22" s="12">
         <v>0.88541666666666663</v>
       </c>
-      <c r="D22" s="68" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="69" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="68" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="69" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="70" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" s="64"/>
-      <c r="J22" s="77"/>
-      <c r="K22" s="65"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1686,7 +1649,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1697,61 +1660,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="73" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="74"/>
-      <c r="K1" s="75"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="43"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="24" t="s">
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="71" t="s">
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="72" t="s">
+      <c r="J2" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="72" t="s">
+      <c r="K2" s="50" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="24" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="51"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1775,12 +1738,12 @@
       <c r="G4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="54"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -1804,15 +1767,17 @@
       <c r="G5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="76">
+      <c r="H5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="47">
         <v>1</v>
       </c>
-      <c r="K5" s="61">
-        <v>0</v>
+      <c r="K5" s="48">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1837,15 +1802,17 @@
       <c r="G6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="18"/>
-      <c r="I6" s="63" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="40">
-        <v>2</v>
-      </c>
-      <c r="K6" s="41">
-        <v>1</v>
+      <c r="H6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="8">
+        <v>3</v>
+      </c>
+      <c r="K6" s="9">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1870,16 +1837,12 @@
       <c r="G7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="40">
-        <v>1</v>
-      </c>
-      <c r="K7" s="41">
-        <v>2</v>
-      </c>
+      <c r="H7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="19"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -1903,10 +1866,12 @@
       <c r="G8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="63"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="41"/>
+      <c r="H8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="19"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1922,10 +1887,10 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="41"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -1937,14 +1902,14 @@
       <c r="C10" s="4">
         <v>0.47569444444444442</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="40"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="63"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="41"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -1956,14 +1921,14 @@
       <c r="C11" s="4">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="40"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="41"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="9"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -1976,13 +1941,13 @@
         <v>0.54513888888888895</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="63"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="41"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="9"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -1998,10 +1963,10 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="41"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -2017,10 +1982,10 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="63"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="41"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="9"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -2033,13 +1998,13 @@
         <v>0.64930555555555558</v>
       </c>
       <c r="D15" s="5"/>
-      <c r="E15" s="6"/>
+      <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="41"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -2051,14 +2016,14 @@
       <c r="C16" s="4">
         <v>0.68402777777777779</v>
       </c>
-      <c r="D16" s="43"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="63"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="41"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="9"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -2071,13 +2036,13 @@
         <v>0.71875</v>
       </c>
       <c r="D17" s="5"/>
-      <c r="E17" s="44"/>
+      <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="63"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="41"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="9"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -2089,24 +2054,14 @@
       <c r="C18" s="4">
         <v>0.75347222222222221</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" s="63"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="41"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="9"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -2130,12 +2085,12 @@
       <c r="G19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I19" s="63"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="41"/>
+      <c r="H19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="19"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="9"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -2147,64 +2102,84 @@
       <c r="C20" s="4">
         <v>0.82291666666666663</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="63"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="41"/>
+      <c r="D20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="19"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="9"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="53">
+      <c r="A21" s="15">
         <v>16</v>
       </c>
-      <c r="B21" s="52">
+      <c r="B21" s="14">
         <v>0.82638888888888884</v>
       </c>
       <c r="C21" s="4">
         <v>0.85763888888888884</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="63"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="41"/>
+      <c r="D21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="19"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="9"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="47">
+      <c r="A22" s="11">
         <v>17</v>
       </c>
-      <c r="B22" s="48">
+      <c r="B22" s="12">
         <v>0.86111111111111116</v>
       </c>
-      <c r="C22" s="48">
+      <c r="C22" s="12">
         <v>0.88541666666666663</v>
       </c>
-      <c r="D22" s="49"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="51"/>
-      <c r="I22" s="64"/>
-      <c r="J22" s="77"/>
-      <c r="K22" s="65"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="K2:K4"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="E3:H3"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="K2:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2215,7 +2190,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:D22"/>
+      <selection activeCell="D10" sqref="D10:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2226,63 +2201,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="73" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="74"/>
-      <c r="K1" s="75"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="30"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="24" t="s">
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="71" t="s">
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="72" t="s">
+      <c r="J2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="72" t="s">
+      <c r="K2" s="27" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="24" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -2307,9 +2282,9 @@
       <c r="H4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -2324,18 +2299,26 @@
       <c r="D5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="76">
-        <v>0</v>
-      </c>
-      <c r="K5" s="61">
+      <c r="E5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="8">
         <v>1</v>
+      </c>
+      <c r="K5" s="9">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2351,18 +2334,26 @@
       <c r="D6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="63" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="40">
-        <v>0</v>
-      </c>
-      <c r="K6" s="41">
-        <v>1</v>
+      <c r="E6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="8">
+        <v>3</v>
+      </c>
+      <c r="K6" s="9">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2378,18 +2369,26 @@
       <c r="D7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="40">
+      <c r="E7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="8">
         <v>1</v>
       </c>
-      <c r="K7" s="41">
-        <v>1</v>
+      <c r="K7" s="9">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2405,13 +2404,21 @@
       <c r="D8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="63"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="41"/>
+      <c r="E8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="19"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -2423,16 +2430,14 @@
       <c r="C9" s="4">
         <v>0.44444444444444442</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="41"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -2447,13 +2452,21 @@
       <c r="D10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="63"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="41"/>
+      <c r="E10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="19"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -2468,13 +2481,21 @@
       <c r="D11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="41"/>
+      <c r="E11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="19"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="9"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -2489,13 +2510,21 @@
       <c r="D12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="63"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="41"/>
+      <c r="E12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="19"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="9"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -2510,13 +2539,21 @@
       <c r="D13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="41"/>
+      <c r="E13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="19"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -2531,13 +2568,21 @@
       <c r="D14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="63"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="41"/>
+      <c r="E14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="19"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="9"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -2552,13 +2597,21 @@
       <c r="D15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="41"/>
+      <c r="E15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="19"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -2570,16 +2623,14 @@
       <c r="C16" s="4">
         <v>0.68402777777777779</v>
       </c>
-      <c r="D16" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="63"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="41"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="9"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -2591,16 +2642,14 @@
       <c r="C17" s="4">
         <v>0.71875</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="44"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="63"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="41"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="9"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -2612,14 +2661,14 @@
       <c r="C18" s="4">
         <v>0.75347222222222221</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="63"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="41"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="9"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -2631,14 +2680,14 @@
       <c r="C19" s="4">
         <v>0.78819444444444453</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="63"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="41"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="9"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -2650,17 +2699,17 @@
       <c r="C20" s="4">
         <v>0.82291666666666663</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="63"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="41"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="9"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="53">
+      <c r="A21" s="15">
         <v>16</v>
       </c>
       <c r="B21" s="4">
@@ -2669,37 +2718,37 @@
       <c r="C21" s="4">
         <v>0.85763888888888884</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="63"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="41"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="9"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="47">
+      <c r="A22" s="11">
         <v>17</v>
       </c>
-      <c r="B22" s="48">
+      <c r="B22" s="12">
         <v>0.86111111111111116</v>
       </c>
-      <c r="C22" s="48">
+      <c r="C22" s="12">
         <v>0.88541666666666663</v>
       </c>
-      <c r="D22" s="49"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="58"/>
-      <c r="I22" s="64"/>
-      <c r="J22" s="77"/>
-      <c r="K22" s="65"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="21"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I23" s="55"/>
-      <c r="J23" s="55"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>